<commit_message>
Roboto font added, minor fixes
</commit_message>
<xml_diff>
--- a/TemplateAudit.xlsx
+++ b/TemplateAudit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egorovchinnikov/PhpstormProjects/ramdom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC2586-6EE1-A54B-838D-44A6C3580C15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDFFE1C-E038-A741-A2F7-FC19EA894995}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19320" windowHeight="13660" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1099,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1137,7 +1137,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="3">
         <f>POWER(SUM(B2, B4), 2)</f>
-        <v>3648100</v>
+        <v>26142769</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>1797</v>
+        <v>5000</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5" t="b">

</xml_diff>